<commit_message>
testes funcionando, plotagem funcionando
</commit_message>
<xml_diff>
--- a/data/exemplos.xlsx
+++ b/data/exemplos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Dunnet"/>
@@ -537,7 +537,7 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -685,7 +685,7 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -694,7 +694,7 @@
     <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,7 +705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -716,7 +716,7 @@
         <v>2.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -727,7 +727,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -738,7 +738,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -749,7 +749,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -760,7 +760,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -771,7 +771,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -782,7 +782,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -793,7 +793,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -804,7 +804,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -815,7 +815,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -826,7 +826,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -837,7 +837,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -848,7 +848,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -859,7 +859,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -870,7 +870,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -881,7 +881,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -892,7 +892,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -903,7 +903,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -914,7 +914,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -925,7 +925,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -936,7 +936,7 @@
         <v>4.9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -947,7 +947,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -958,7 +958,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>